<commit_message>
2e kans - 3 Lotte Houwen
</commit_message>
<xml_diff>
--- a/TestScriptLotteHouwen(Blok2.6).xlsx
+++ b/TestScriptLotteHouwen(Blok2.6).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Step</t>
   </si>
@@ -105,58 +105,34 @@
     <t>Lotte Houwen</t>
   </si>
   <si>
-    <t>bestand inlezen: .fasta bestand meegeven</t>
-  </si>
-  <si>
-    <t>bestand inlezen: .pdf bestand meegeven</t>
-  </si>
-  <si>
-    <t>bestand inlezen: .doc (Word) bestand meegeven</t>
-  </si>
-  <si>
-    <t>bestand inlezen: .png bestand meegeven</t>
-  </si>
-  <si>
-    <t>IndexOutOfBounce exception</t>
-  </si>
-  <si>
     <t>Geen exception. Bestand is in te lezen en kan nu gefilterd en gesorteerd gaan worden.</t>
   </si>
   <si>
     <t>bestand inlezen: virushostdb.tsv meegeven</t>
   </si>
   <si>
-    <t>Bestand ophalen File teksveld</t>
-  </si>
-  <si>
     <t>Er gebeurd niets</t>
   </si>
   <si>
     <t>dezelfde lijsten terug, op dezelfde volgorde en bij overeenkomst alle virussen terug die bij de 2 tekstarea's staan.</t>
   </si>
   <si>
-    <t>In elk tekstarea een eigen lijst van virusid bij overeenkomst geen output.</t>
-  </si>
-  <si>
-    <t>Filteren/Sorteren: bij classe Yellow fever virus group en bij host 10090 en 10090 (dezelfde hosts)</t>
-  </si>
-  <si>
-    <t>Filteren/Sorteren: bij classe Yellow fever group en bij host 10090 en 100937 ( niet dezelfde hosts)</t>
-  </si>
-  <si>
-    <t>Filteren/Sorteren: bij classe Yello fever group en bij host 10090 en 7158 (niet dezelfde hosts)</t>
-  </si>
-  <si>
     <t>In elk tekstarea een eigen lijst van virusid bij overeenkomst 1 overeenkomstige virusid</t>
   </si>
   <si>
-    <t>De eerste area kent geen virushost toegewezen. Dus ook geen overeenkomsten</t>
-  </si>
-  <si>
-    <t>Filteren/Sorteren: bij classe unclassified Chysovirus en bij host 1405299 en 318829 ( niet dezelfde hosts)</t>
-  </si>
-  <si>
-    <t>Filteren/Sorteren: bij classe  unclassified Chysovirus en bij host 55169 en 318829 (niet dezelfde hosts)</t>
+    <t>Filteren/Sorteren: bij classe ssRNA virusses en bij host 9796 en 9796 (dezelfde hosts)</t>
+  </si>
+  <si>
+    <t>Filteren/Sorteren: bij classe ssRNA virusses en bij host 9796 en 9790 (dezelfde hosts)</t>
+  </si>
+  <si>
+    <t>sorteeroptie virusid</t>
+  </si>
+  <si>
+    <t>Bestand dmv typen invoeren in bestandveld</t>
+  </si>
+  <si>
+    <t>20:0000</t>
   </si>
 </sst>
 </file>
@@ -216,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -593,19 +569,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -654,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -776,27 +739,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -811,6 +766,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1158,7 +1115,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1169,7 +1126,7 @@
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" customWidth="1"/>
     <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1193,11 +1150,11 @@
       <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
@@ -1206,13 +1163,13 @@
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1220,13 +1177,13 @@
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1234,13 +1191,13 @@
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1248,13 +1205,13 @@
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1271,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="17">
-        <v>43138</v>
+        <v>43159</v>
       </c>
       <c r="H7" s="18"/>
     </row>
@@ -1286,8 +1243,8 @@
       <c r="F8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="35">
-        <v>0.88194444444444453</v>
+      <c r="G8" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="H8" s="24"/>
     </row>
@@ -1310,38 +1267,38 @@
       <c r="F9" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="49"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="53"/>
+    </row>
+    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>1</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>2</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>19</v>
@@ -1356,25 +1313,27 @@
         <v>3</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>4</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>28</v>
@@ -1384,22 +1343,16 @@
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
-      <c r="G13" s="36"/>
+      <c r="G13" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
-        <v>5</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="36"/>
@@ -1409,107 +1362,69 @@
       <c r="A15" s="28">
         <v>6</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
       <c r="G15" s="36"/>
       <c r="H15" s="37"/>
     </row>
-    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="28">
         <v>7</v>
       </c>
-      <c r="B16" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="36"/>
       <c r="H16" s="37"/>
     </row>
-    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="28">
         <v>8</v>
       </c>
-      <c r="B17" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="36"/>
       <c r="H17" s="37"/>
     </row>
-    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="28">
         <v>9</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="36"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="28">
         <v>10</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>34</v>
-      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="30"/>
-      <c r="E19" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="E19" s="30"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="36" t="s">
-        <v>39</v>
-      </c>
+      <c r="G19" s="36"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="28">
         <v>11</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>19</v>
-      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="36"/>
@@ -1632,11 +1547,28 @@
       <c r="D30" s="34"/>
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="57"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -1649,23 +1581,6 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>